<commit_message>
handling excel and hashmap example
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Books.xlsx
+++ b/src/test/resources/data/Books.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7830" activeTab="1"/>
+    <workbookView windowWidth="20490" windowHeight="7830" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="bookDetails" sheetId="2" r:id="rId2"/>
+    <sheet name="RestAssured" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
   <si>
     <t>Testcases</t>
   </si>
@@ -183,6 +184,102 @@
   </si>
   <si>
     <t>Testuser8</t>
+  </si>
+  <si>
+    <t>javaApi21</t>
+  </si>
+  <si>
+    <t>java-12</t>
+  </si>
+  <si>
+    <t>RA22</t>
+  </si>
+  <si>
+    <t>Testuser22</t>
+  </si>
+  <si>
+    <t>javaApi22</t>
+  </si>
+  <si>
+    <t>java-13</t>
+  </si>
+  <si>
+    <t>RA23</t>
+  </si>
+  <si>
+    <t>Testuser23</t>
+  </si>
+  <si>
+    <t>javaApi23</t>
+  </si>
+  <si>
+    <t>java-14</t>
+  </si>
+  <si>
+    <t>RA24</t>
+  </si>
+  <si>
+    <t>Testuser24</t>
+  </si>
+  <si>
+    <t>javaApi24</t>
+  </si>
+  <si>
+    <t>java-15</t>
+  </si>
+  <si>
+    <t>RA25</t>
+  </si>
+  <si>
+    <t>Testuser25</t>
+  </si>
+  <si>
+    <t>javaApi25</t>
+  </si>
+  <si>
+    <t>java-16</t>
+  </si>
+  <si>
+    <t>RA26</t>
+  </si>
+  <si>
+    <t>Testuser26</t>
+  </si>
+  <si>
+    <t>javaApi26</t>
+  </si>
+  <si>
+    <t>java-17</t>
+  </si>
+  <si>
+    <t>RA27</t>
+  </si>
+  <si>
+    <t>Testuser27</t>
+  </si>
+  <si>
+    <t>javaApi27</t>
+  </si>
+  <si>
+    <t>java-18</t>
+  </si>
+  <si>
+    <t>RA28</t>
+  </si>
+  <si>
+    <t>Testuser28</t>
+  </si>
+  <si>
+    <t>javaApi28</t>
+  </si>
+  <si>
+    <t>java-19</t>
+  </si>
+  <si>
+    <t>RA29</t>
+  </si>
+  <si>
+    <t>Testuser29</t>
   </si>
 </sst>
 </file>
@@ -190,10 +287,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -201,6 +298,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -212,23 +317,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -244,9 +348,55 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -258,9 +408,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -275,74 +439,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -357,187 +454,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -551,11 +648,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -564,7 +667,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -580,17 +683,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -619,6 +711,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -634,17 +735,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -653,148 +750,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -802,10 +899,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1233,8 +1330,8 @@
   <sheetPr/>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="A1:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="3"/>
@@ -1244,10 +1341,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C1" t="s">
@@ -1258,10 +1355,10 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C2" t="s">
@@ -1272,10 +1369,10 @@
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C3" t="s">
@@ -1286,10 +1383,10 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C4" t="s">
@@ -1300,10 +1397,10 @@
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C5" t="s">
@@ -1314,10 +1411,10 @@
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C6" t="s">
@@ -1328,10 +1425,10 @@
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C7" t="s">
@@ -1342,10 +1439,10 @@
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>53</v>
       </c>
       <c r="C8" t="s">
@@ -1377,4 +1474,154 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="$A1:$XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="3"/>
+  <cols>
+    <col min="4" max="4" width="15.5714285714286" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" display="javaApi21"/>
+    <hyperlink ref="B1" r:id="rId2" display="java-12" tooltip="mailto:vinisoft@123"/>
+    <hyperlink ref="A2" r:id="rId1" display="javaApi22"/>
+    <hyperlink ref="A3" r:id="rId1" display="javaApi23"/>
+    <hyperlink ref="A4" r:id="rId1" display="javaApi24"/>
+    <hyperlink ref="A5" r:id="rId1" display="javaApi25"/>
+    <hyperlink ref="A6" r:id="rId1" display="javaApi26"/>
+    <hyperlink ref="A7" r:id="rId1" display="javaApi27"/>
+    <hyperlink ref="A8" r:id="rId1" display="javaApi28"/>
+    <hyperlink ref="B2" r:id="rId2" display="java-13" tooltip="mailto:vinisoft@123"/>
+    <hyperlink ref="B3" r:id="rId2" display="java-14" tooltip="mailto:vinisoft@123"/>
+    <hyperlink ref="B4" r:id="rId2" display="java-15" tooltip="mailto:vinisoft@123"/>
+    <hyperlink ref="B5" r:id="rId2" display="java-16" tooltip="mailto:vinisoft@123"/>
+    <hyperlink ref="B6" r:id="rId2" display="java-17" tooltip="mailto:vinisoft@123"/>
+    <hyperlink ref="B7" r:id="rId2" display="java-18" tooltip="mailto:vinisoft@123"/>
+    <hyperlink ref="B8" r:id="rId2" display="java-19" tooltip="mailto:vinisoft@123"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>